<commit_message>
h- updated log file
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bead1d9252beea6e/Desktop/restaurant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{5425CA62-8525-410C-BF58-AC118E7F8316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9660B36B-A130-4BA7-B1A1-DD35A2356C4D}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{5425CA62-8525-410C-BF58-AC118E7F8316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A177BA30-C37A-4AF5-BB44-08F663FD8660}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B94B14EE-90B1-4BFA-A8F6-382603C3EF04}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -118,6 +118,51 @@
   </si>
   <si>
     <t>added styling to the Contact page</t>
+  </si>
+  <si>
+    <t>created sendmessage page and styling</t>
+  </si>
+  <si>
+    <t>created book a table page and styling</t>
+  </si>
+  <si>
+    <t>created confirmation page and styling</t>
+  </si>
+  <si>
+    <t>created common css file</t>
+  </si>
+  <si>
+    <t>11-25-2023</t>
+  </si>
+  <si>
+    <t>created documentation and finalising the home page</t>
+  </si>
+  <si>
+    <t>created documentation and finalising the About us page</t>
+  </si>
+  <si>
+    <t>created documentation and finalising the Menu page</t>
+  </si>
+  <si>
+    <t>created documentation and finalising the Contact us page</t>
+  </si>
+  <si>
+    <t>12-03-2023</t>
+  </si>
+  <si>
+    <t>12-01-2023</t>
+  </si>
+  <si>
+    <t>updated styling and responsivenss to the Home page</t>
+  </si>
+  <si>
+    <t>updated styling and responsivenss to the About us page</t>
+  </si>
+  <si>
+    <t>updated styling and responsivenss to the Menu page</t>
+  </si>
+  <si>
+    <t>updated styling and responsivenss to the Contact page</t>
   </si>
 </sst>
 </file>
@@ -484,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEC7F2B-7E61-4156-BE43-EE6458CBFC96}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,6 +733,138 @@
         <v>25</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>